<commit_message>
update bases on the requirement
</commit_message>
<xml_diff>
--- a/documents/问题需求整理.xlsx
+++ b/documents/问题需求整理.xlsx
@@ -9,14 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14400" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14400" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="问题整理" sheetId="1" r:id="rId1"/>
     <sheet name="流程" sheetId="2" r:id="rId2"/>
-    <sheet name="Index" sheetId="3" r:id="rId3"/>
-    <sheet name="CreateMatch" sheetId="4" r:id="rId4"/>
-    <sheet name="CreateMatchSuccess" sheetId="5" r:id="rId5"/>
+    <sheet name="Login" sheetId="8" r:id="rId3"/>
+    <sheet name="Index" sheetId="3" r:id="rId4"/>
+    <sheet name="CreateMatch" sheetId="4" r:id="rId5"/>
+    <sheet name="CreateMatchSuccess" sheetId="5" r:id="rId6"/>
+    <sheet name="CreateGameRule" sheetId="6" r:id="rId7"/>
+    <sheet name="GameRuleList" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="143">
   <si>
     <t>新建赛事</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -332,267 +335,259 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>只有小组淘汰赛有</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数字类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>确认（按钮）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直接淘汰赛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Item</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>联赛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A-球队数量总数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A1A2B1B2----最大字母为球队数量总数/2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小组淘汰赛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">A1-A（球队数量总数/小组数量）最大字母为小组数量总数  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>例子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>直接淘汰赛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A1A2B1B2C1C2D1D4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小组淘汰赛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A1A2A3A4 B1B2B3B4 C1C2C3C4  D1D2D3D4 E1E2E3E4 F1F2F3F4 G1G2G3G4 H1H2H3H4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ABCDEFGHIJKL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>匹配球队（按钮）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>说明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>进入匹配页面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>球队匹配</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>组名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>球队名（列表形式）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>赛区（列表形式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>保存（按钮）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>赛程创建（按钮）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建赛程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主队</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>客队</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示球队队名和组名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>饼子队-A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>场地</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>类型</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小组赛，淘汰赛，16强，8强，4强，冠军赛，季军赛，总决赛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>年月日</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加（按钮）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更新（按钮）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看赛程（按钮）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>赛程查看</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一步</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第二步</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第三步</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第四步</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对战</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>详情</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>未开战，进行中，已结束</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>链接</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>详情页面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>比赛数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>比赛关联队报</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>打算加个球队管理</t>
+  </si>
+  <si>
+    <t>状态</t>
+  </si>
+  <si>
+    <t>用户头像下拉列表里加上比赛规则管理</t>
+  </si>
+  <si>
     <t>直接淘汰赛/小组淘汰赛/联赛</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>小组数量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>只有小组淘汰赛有</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>输入球队数量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>数字类型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>确认（按钮）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>球队分组</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>直接淘汰赛</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Item</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Value</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>联赛</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A-球队数量总数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A1A2B1B2----最大字母为球队数量总数/2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>小组淘汰赛</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">A1-A（球队数量总数/小组数量）最大字母为小组数量总数  </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>例子</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>直接淘汰赛</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A1A2B1B2C1C2D1D4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>小组淘汰赛</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A1A2A3A4 B1B2B3B4 C1C2C3C4  D1D2D3D4 E1E2E3E4 F1F2F3F4 G1G2G3G4 H1H2H3H4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ABCDEFGHIJKL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>匹配球队（按钮）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>说明</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>进入匹配页面</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>球队匹配</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>组名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>球队名（列表形式）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>赛区（列表形式</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>保存（按钮）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>赛程创建（按钮）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>创建赛程</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>主队</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>客队</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>显示球队队名和组名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>饼子队-A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>日期</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>地点</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>场地</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>类型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>小组赛，淘汰赛，16强，8强，4强，冠军赛，季军赛，总决赛</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>列表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>年月日</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>添加（按钮）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>更新（按钮）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>查看赛程（按钮）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>赛程查看</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>匹配球队</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>第一步</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>第二步</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>第三步</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>第四步</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>时间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>对战</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>状态</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>详情</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>未开战，进行中，已结束</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>链接</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>详情页面</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>比赛数据</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>比赛关联队报</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>返回</t>
-  </si>
-  <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>打算加个球队管理</t>
-  </si>
-  <si>
-    <t>状态</t>
-  </si>
-  <si>
-    <t>用户头像下拉列表里加上比赛规则管理</t>
+  </si>
+  <si>
+    <t>赛制列表</t>
   </si>
 </sst>
 </file>
@@ -694,7 +689,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -718,20 +713,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="11"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="11"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -916,6 +914,135 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>236295</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>160955</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="400050"/>
+          <a:ext cx="14638095" cy="7761905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>236295</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>160955</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="400050"/>
+          <a:ext cx="14638095" cy="7761905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>236295</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>160955</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="400050"/>
+          <a:ext cx="14638095" cy="7761905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1282,8 +1409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1303,7 +1430,7 @@
         <v>5</v>
       </c>
       <c r="I3" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="4:9">
@@ -1316,8 +1443,8 @@
       <c r="F4" t="s">
         <v>2</v>
       </c>
-      <c r="I4" s="17" t="s">
-        <v>143</v>
+      <c r="I4" s="14" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="4:9">
@@ -1327,35 +1454,35 @@
       <c r="F5" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="17" t="s">
-        <v>140</v>
+      <c r="I5" s="14" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="4:9">
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14" t="s">
+      <c r="E6" s="12"/>
+      <c r="F6" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="16" t="s">
-        <v>141</v>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="15" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="4:9">
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14" t="s">
+      <c r="E7" s="12"/>
+      <c r="F7" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="16"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1375,8 +1502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:P78"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1399,7 +1526,7 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="11" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1407,7 +1534,7 @@
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="11" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1415,7 +1542,7 @@
       <c r="B7">
         <v>3</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="11" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1423,7 +1550,7 @@
       <c r="B8">
         <v>4</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="11" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1858,41 +1985,44 @@
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
-      <c r="J34" s="15"/>
+      <c r="J34" s="13"/>
       <c r="K34" s="1"/>
       <c r="L34" s="6"/>
       <c r="M34" s="1"/>
     </row>
     <row r="35" spans="2:13">
       <c r="B35" t="s">
-        <v>126</v>
-      </c>
-      <c r="C35" t="s">
+        <v>121</v>
+      </c>
+      <c r="C35" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D35" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="E35" s="11"/>
+      <c r="E35" s="17"/>
       <c r="F35" s="1"/>
-      <c r="J35" s="15"/>
+      <c r="J35" s="13"/>
       <c r="K35" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="L35" s="6"/>
       <c r="M35" s="1"/>
     </row>
     <row r="36" spans="2:13">
+      <c r="C36" s="11" t="s">
+        <v>142</v>
+      </c>
       <c r="D36" s="7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="J36" s="15"/>
+        <v>95</v>
+      </c>
+      <c r="J36" s="13"/>
       <c r="K36" s="1"/>
       <c r="L36" s="6"/>
       <c r="M36" s="1"/>
@@ -1905,7 +2035,7 @@
         <v>74</v>
       </c>
       <c r="F37" s="1"/>
-      <c r="J37" s="15"/>
+      <c r="J37" s="13"/>
       <c r="K37" s="1"/>
       <c r="L37" s="6"/>
       <c r="M37" s="1"/>
@@ -1915,29 +2045,29 @@
         <v>76</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>77</v>
+        <v>139</v>
       </c>
       <c r="F38" s="1"/>
-      <c r="J38" s="15"/>
+      <c r="J38" s="13"/>
       <c r="K38" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="L38" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="2:13">
       <c r="D39" s="1" t="s">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="E39" s="8"/>
       <c r="F39" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="J39" s="15"/>
+        <v>77</v>
+      </c>
+      <c r="J39" s="13"/>
       <c r="K39" s="1"/>
       <c r="L39" s="6">
         <v>8</v>
@@ -1946,13 +2076,13 @@
     </row>
     <row r="40" spans="2:13">
       <c r="D40" s="1" t="s">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F40" s="1"/>
-      <c r="J40" s="15"/>
+      <c r="J40" s="13"/>
       <c r="K40" s="1">
         <v>8</v>
       </c>
@@ -1964,62 +2094,62 @@
       </c>
     </row>
     <row r="41" spans="2:13">
-      <c r="D41" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="J41" s="15"/>
+      <c r="D41" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="J41" s="13"/>
       <c r="K41" s="1"/>
       <c r="L41" s="6"/>
       <c r="M41" s="1"/>
     </row>
     <row r="42" spans="2:13" ht="126">
       <c r="D42" s="1" t="s">
-        <v>83</v>
+        <v>141</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="J42" s="15"/>
+        <v>80</v>
+      </c>
+      <c r="J42" s="13"/>
       <c r="K42" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="M42" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43" spans="2:13">
       <c r="D43" s="1"/>
       <c r="E43" s="8" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="2:13" ht="47.25">
       <c r="D44" s="1"/>
       <c r="E44" s="8" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45" spans="2:13">
-      <c r="D45" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="E45" s="11"/>
+      <c r="D45" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="E45" s="17"/>
       <c r="F45" s="9" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="46" spans="2:13">
@@ -2027,26 +2157,24 @@
     </row>
     <row r="47" spans="2:13">
       <c r="B47" t="s">
-        <v>127</v>
-      </c>
-      <c r="C47" t="s">
-        <v>125</v>
-      </c>
-      <c r="D47" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
+        <v>122</v>
+      </c>
+      <c r="C47" s="18"/>
+      <c r="D47" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
     </row>
     <row r="48" spans="2:13">
       <c r="D48" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49" spans="2:7">
@@ -2076,85 +2204,86 @@
     </row>
     <row r="54" spans="2:7">
       <c r="D54" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F54" s="1"/>
     </row>
     <row r="56" spans="2:7">
       <c r="B56" t="s">
-        <v>128</v>
-      </c>
-      <c r="D56" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
+        <v>123</v>
+      </c>
+      <c r="C56" s="18"/>
+      <c r="D56" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
     </row>
     <row r="57" spans="2:7">
       <c r="D57" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G57" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="58" spans="2:7">
       <c r="D58" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="59" spans="2:7">
       <c r="D59" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="60" spans="2:7">
       <c r="D60" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E60" s="1"/>
       <c r="F60" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="61" spans="2:7">
       <c r="D61" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
     </row>
     <row r="62" spans="2:7">
       <c r="D62" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
     </row>
     <row r="63" spans="2:7" ht="31.5">
       <c r="D63" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E63" s="10" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="64" spans="2:7">
@@ -2164,91 +2293,91 @@
     </row>
     <row r="65" spans="2:6">
       <c r="D65" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="67" spans="2:6">
       <c r="B67" t="s">
-        <v>129</v>
-      </c>
-      <c r="D67" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="E67" s="12"/>
-      <c r="F67" s="12"/>
+      <c r="D67" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="E67" s="16"/>
+      <c r="F67" s="16"/>
     </row>
     <row r="68" spans="2:6">
       <c r="D68" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
     </row>
     <row r="69" spans="2:6">
       <c r="D69" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
     </row>
     <row r="70" spans="2:6">
       <c r="D70" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
     </row>
     <row r="71" spans="2:6">
       <c r="D71" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
     </row>
     <row r="72" spans="2:6">
       <c r="D72" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
     </row>
     <row r="73" spans="2:6">
       <c r="D73" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F73" s="1"/>
     </row>
     <row r="74" spans="2:6">
       <c r="D74" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F74" s="1"/>
     </row>
     <row r="76" spans="2:6">
       <c r="D76" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="77" spans="2:6">
       <c r="D77" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="78" spans="2:6">
       <c r="D78" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2265,6 +2394,9 @@
     <hyperlink ref="C6" location="Index!A1" display="显示本用户关联的信息"/>
     <hyperlink ref="C7" location="CreateMatch!A1" display="创建一个新的赛事"/>
     <hyperlink ref="C8" location="CreateMatchSuccess!A1" display="添加赛事信息"/>
+    <hyperlink ref="C35" location="CreateGameRule!A1" display="先创建赛制"/>
+    <hyperlink ref="C36" location="GameRuleList!A1" display="赛制列表"/>
+    <hyperlink ref="C5" location="Login!A1" display="登录"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -2287,13 +2419,13 @@
   <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="2:2">
-      <c r="B1" s="13" t="s">
-        <v>139</v>
+      <c r="B1" s="11" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" location="工作表2!A1" display="返回"/>
+    <hyperlink ref="B1" location="流程!A1" display="返回"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2311,8 +2443,8 @@
   <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="2:2">
-      <c r="B1" s="13" t="s">
-        <v>139</v>
+      <c r="B1" s="11" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2328,6 +2460,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1"/>
   <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="2:2">
+      <c r="B1" s="11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" location="工作表2!A1" display="返回"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
@@ -2335,8 +2491,8 @@
   <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="2:2">
-      <c r="B1" s="13" t="s">
-        <v>139</v>
+      <c r="B1" s="11" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2346,4 +2502,52 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="2:2">
+      <c r="B1" s="11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" location="流程!A1" display="返回"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="2:2">
+      <c r="B1" s="11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" location="流程!A1" display="返回"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add game time table
</commit_message>
<xml_diff>
--- a/documents/问题需求整理.xlsx
+++ b/documents/问题需求整理.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22935" windowHeight="10530" tabRatio="500"/>
+    <workbookView windowWidth="22935" windowHeight="10950" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="问题整理" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116">
   <si>
     <t>页面</t>
   </si>
@@ -74,10 +74,16 @@
     <t>用vs2015生成数据库时总是生成之前有的多余的列</t>
   </si>
   <si>
+    <t>创建表的Model不能被继承</t>
+  </si>
+  <si>
     <t>由于改了model，删除了一些字段，然后现在查询list都报错说没有那些列</t>
   </si>
   <si>
     <t>表关联查询结果不会处理</t>
+  </si>
+  <si>
+    <t>赛区哪儿来的？</t>
   </si>
   <si>
     <t>Step</t>
@@ -370,12 +376,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -401,36 +407,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -460,21 +436,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -482,14 +452,29 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -528,6 +513,35 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -549,6 +563,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -573,25 +611,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -639,12 +701,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -664,48 +720,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -778,30 +792,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -855,152 +845,179 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="48">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1038,7 +1055,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="48">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
     <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
@@ -1048,45 +1065,46 @@
     <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
     <cellStyle name="差" xfId="7" builtinId="27"/>
     <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="超链接" xfId="9" builtinId="8"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="10" builtinId="40"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
     <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="注释" xfId="12" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="13" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="14" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="15" builtinId="11"/>
-    <cellStyle name="标题" xfId="16" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="17" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="18" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="19" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="20" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="21" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="22" builtinId="44"/>
-    <cellStyle name="输出" xfId="23" builtinId="21"/>
-    <cellStyle name="计算" xfId="24" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="25" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="26" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="27" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="28" builtinId="24"/>
-    <cellStyle name="汇总" xfId="29" builtinId="25"/>
-    <cellStyle name="好" xfId="30" builtinId="26"/>
-    <cellStyle name="适中" xfId="31" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="32" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="33" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="34" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="35" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="36" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="37" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="38" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="39" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="40" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="41" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="42" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="46" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="47" builtinId="52"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
@@ -1673,14 +1691,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="D3:I12"/>
+  <dimension ref="D3:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
   <cols>
+    <col min="4" max="4" width="19.75" customWidth="1"/>
     <col min="6" max="6" width="15.5" customWidth="1"/>
     <col min="9" max="9" width="35.625" customWidth="1"/>
   </cols>
@@ -1750,24 +1769,35 @@
       <c r="H7" s="15"/>
       <c r="I7" s="17"/>
     </row>
-    <row r="10" spans="4:4">
+    <row r="10" spans="4:9">
       <c r="D10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="4:4">
+      <c r="I10" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="4:9">
       <c r="D11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="4:4">
+        <v>18</v>
+      </c>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="4:9">
       <c r="D12" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="I12" s="9"/>
+    </row>
+    <row r="14" spans="4:4">
+      <c r="D14" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="I6:I7"/>
+    <mergeCell ref="I10:I12"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1779,8 +1809,8 @@
   <sheetPr/>
   <dimension ref="B4:P78"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -1796,7 +1826,7 @@
   <sheetData>
     <row r="4" spans="3:3">
       <c r="C4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="2:3">
@@ -1804,7 +1834,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="2:3">
@@ -1812,7 +1842,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="2:3">
@@ -1820,7 +1850,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="2:3">
@@ -1828,7 +1858,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="2:3">
@@ -1836,23 +1866,23 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="4:5">
       <c r="D10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="4:5">
       <c r="D11" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="3:15">
@@ -1865,7 +1895,7 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
@@ -1875,47 +1905,47 @@
     <row r="14" spans="3:15">
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L14" s="12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="M14" s="12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="N14" s="12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="O14" s="12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="3:15">
       <c r="C15" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -1923,7 +1953,7 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="L15" s="12"/>
       <c r="M15" s="12">
@@ -1931,16 +1961,16 @@
       </c>
       <c r="N15" s="3"/>
       <c r="O15" s="13" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="3:16">
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -1948,7 +1978,7 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="12" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L16" s="12">
         <v>8</v>
@@ -1960,19 +1990,19 @@
         <v>4</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="P16" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="3:15">
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -1980,7 +2010,7 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L17" s="12"/>
       <c r="M17" s="12">
@@ -1988,7 +2018,7 @@
       </c>
       <c r="N17" s="3"/>
       <c r="O17" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="3:15">
@@ -2008,16 +2038,16 @@
     </row>
     <row r="19" spans="3:15">
       <c r="C19" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
@@ -2030,24 +2060,24 @@
     <row r="20" spans="3:15">
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="12" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
@@ -2061,14 +2091,14 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="4" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="J21" s="3"/>
       <c r="K21" s="12" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
@@ -2077,7 +2107,7 @@
     </row>
     <row r="22" spans="3:15">
       <c r="C22" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -2095,19 +2125,19 @@
     <row r="23" spans="3:15">
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
@@ -2124,7 +2154,7 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
@@ -2136,7 +2166,7 @@
     </row>
     <row r="25" spans="3:15">
       <c r="C25" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -2154,7 +2184,7 @@
     <row r="26" spans="3:15">
       <c r="C26" s="3"/>
       <c r="D26" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -2171,7 +2201,7 @@
     <row r="27" spans="3:15">
       <c r="C27" s="3"/>
       <c r="D27" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -2188,7 +2218,7 @@
     <row r="28" spans="3:15">
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -2205,7 +2235,7 @@
     <row r="29" spans="3:15">
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -2222,7 +2252,7 @@
     <row r="30" spans="3:15">
       <c r="C30" s="3"/>
       <c r="D30" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -2239,7 +2269,7 @@
     <row r="31" spans="3:15">
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -2255,10 +2285,10 @@
     </row>
     <row r="34" spans="3:13">
       <c r="C34" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
@@ -2269,35 +2299,35 @@
     </row>
     <row r="35" spans="2:13">
       <c r="B35" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="3"/>
       <c r="J35" s="14"/>
       <c r="K35" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="L35" s="4"/>
       <c r="M35" s="3"/>
     </row>
     <row r="36" spans="3:13">
       <c r="C36" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J36" s="14"/>
       <c r="K36" s="3"/>
@@ -2306,10 +2336,10 @@
     </row>
     <row r="37" spans="4:13">
       <c r="D37" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F37" s="3"/>
       <c r="J37" s="14"/>
@@ -2319,30 +2349,30 @@
     </row>
     <row r="38" spans="4:13">
       <c r="D38" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F38" s="3"/>
       <c r="J38" s="14"/>
       <c r="K38" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="4:13">
       <c r="D39" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E39" s="6"/>
       <c r="F39" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J39" s="14"/>
       <c r="K39" s="3"/>
@@ -2353,10 +2383,10 @@
     </row>
     <row r="40" spans="4:13">
       <c r="D40" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F40" s="3"/>
       <c r="J40" s="14"/>
@@ -2372,7 +2402,7 @@
     </row>
     <row r="41" spans="4:13">
       <c r="D41" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
@@ -2383,50 +2413,50 @@
     </row>
     <row r="42" ht="114" spans="4:13">
       <c r="D42" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="J42" s="14"/>
       <c r="K42" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="L42" s="6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="M42" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="4:6">
       <c r="D43" s="3"/>
       <c r="E43" s="6" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" ht="28.5" spans="4:6">
       <c r="D44" s="3"/>
       <c r="E44" s="6" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="4:6">
       <c r="D45" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E45" s="5"/>
       <c r="F45" s="7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" spans="5:5">
@@ -2434,24 +2464,24 @@
     </row>
     <row r="47" spans="2:6">
       <c r="B47" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C47" s="9"/>
       <c r="D47" s="10" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
     </row>
     <row r="48" spans="4:6">
       <c r="D48" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="4:6">
@@ -2481,86 +2511,86 @@
     </row>
     <row r="54" spans="4:6">
       <c r="D54" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F54" s="3"/>
     </row>
     <row r="56" spans="2:6">
       <c r="B56" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C56" s="9"/>
       <c r="D56" s="10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E56" s="10"/>
       <c r="F56" s="10"/>
     </row>
     <row r="57" spans="4:7">
       <c r="D57" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E57" s="3"/>
       <c r="F57" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G57" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="58" spans="4:6">
       <c r="D58" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E58" s="3"/>
       <c r="F58" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="4:6">
       <c r="D59" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E59" s="3"/>
       <c r="F59" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="60" spans="4:6">
       <c r="D60" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="4:6">
       <c r="D61" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
     </row>
     <row r="62" spans="4:6">
       <c r="D62" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
     </row>
     <row r="63" ht="28.5" spans="4:6">
       <c r="D63" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E63" s="11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="64" spans="4:6">
@@ -2570,56 +2600,56 @@
     </row>
     <row r="65" spans="4:6">
       <c r="D65" s="3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="67" spans="2:6">
       <c r="B67" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E67" s="10"/>
       <c r="F67" s="10"/>
     </row>
     <row r="68" spans="4:6">
       <c r="D68" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
     </row>
     <row r="69" spans="4:6">
       <c r="D69" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
     </row>
     <row r="70" spans="4:6">
       <c r="D70" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
     </row>
     <row r="71" spans="4:6">
       <c r="D71" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
     </row>
     <row r="72" spans="4:6">
       <c r="D72" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
@@ -2629,32 +2659,32 @@
         <v>3</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F73" s="3"/>
     </row>
     <row r="74" spans="4:6">
       <c r="D74" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F74" s="3"/>
     </row>
     <row r="76" spans="4:4">
       <c r="D76" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="77" spans="4:4">
       <c r="D77" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="78" spans="4:4">
       <c r="D78" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2693,7 +2723,7 @@
   <sheetData>
     <row r="1" spans="2:2">
       <c r="B1" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2719,7 +2749,7 @@
   <sheetData>
     <row r="1" spans="2:2">
       <c r="B1" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2745,7 +2775,7 @@
   <sheetData>
     <row r="1" spans="2:2">
       <c r="B1" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2771,7 +2801,7 @@
   <sheetData>
     <row r="1" spans="2:2">
       <c r="B1" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2797,7 +2827,7 @@
   <sheetData>
     <row r="1" spans="2:2">
       <c r="B1" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2823,7 +2853,7 @@
   <sheetData>
     <row r="1" spans="2:2">
       <c r="B1" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>